<commit_message>
ajustes con nuevas directrices
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
@@ -304,9 +304,6 @@
     <t xml:space="preserve">El triunfo de Madero </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: El Plan Ayala</t>
-  </si>
-  <si>
     <t xml:space="preserve">La reacción a los planes campesinos </t>
   </si>
   <si>
@@ -395,9 +392,6 @@
   </si>
   <si>
     <t>Estado Novo de Brasil</t>
-  </si>
-  <si>
-    <t>Practica: Las características del populismo</t>
   </si>
   <si>
     <t>Ejercicio que sintetiza las características del populismo latinoamericano</t>
@@ -531,6 +525,12 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>El Plan Ayala</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El populismo en América Latina</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1206,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1309,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>87</v>
@@ -1341,7 +1341,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>87</v>
@@ -1375,7 +1375,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>87</v>
@@ -1409,7 +1409,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>87</v>
@@ -1424,7 +1424,7 @@
         <v>93</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="H5" s="37">
         <v>1</v>
@@ -1433,7 +1433,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K5" s="45" t="s">
         <v>69</v>
@@ -1445,7 +1445,7 @@
         <v>62</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O5" s="44" t="s">
         <v>19</v>
@@ -1461,7 +1461,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>87</v>
@@ -1473,7 +1473,7 @@
         <v>90</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
@@ -1495,7 +1495,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>87</v>
@@ -1507,7 +1507,7 @@
         <v>90</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
@@ -1529,7 +1529,7 @@
         <v>66</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>87</v>
@@ -1541,10 +1541,10 @@
         <v>90</v>
       </c>
       <c r="F8" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="36" t="s">
         <v>97</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>98</v>
       </c>
       <c r="H8" s="37">
         <v>2</v>
@@ -1553,7 +1553,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K8" s="45" t="s">
         <v>69</v>
@@ -1565,7 +1565,7 @@
         <v>85</v>
       </c>
       <c r="N8" s="47" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>19</v>
@@ -1581,7 +1581,7 @@
         <v>66</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>87</v>
@@ -1593,7 +1593,7 @@
         <v>90</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="37"/>
@@ -1615,7 +1615,7 @@
         <v>66</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>87</v>
@@ -1627,7 +1627,7 @@
         <v>90</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="37"/>
@@ -1649,7 +1649,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>87</v>
@@ -1661,7 +1661,7 @@
         <v>90</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="37"/>
@@ -1683,7 +1683,7 @@
         <v>66</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>87</v>
@@ -1692,18 +1692,18 @@
         <v>88</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="37">
         <v>3</v>
       </c>
       <c r="I12" s="37"/>
       <c r="J12" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K12" s="45" t="s">
         <v>69</v>
@@ -1715,7 +1715,7 @@
         <v>43</v>
       </c>
       <c r="N12" s="47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>19</v>
@@ -1731,7 +1731,7 @@
         <v>66</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>87</v>
@@ -1740,18 +1740,18 @@
         <v>88</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="30"/>
       <c r="G13" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="37">
         <v>4</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="45" t="s">
         <v>69</v>
@@ -1763,7 +1763,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>19</v>
@@ -1779,19 +1779,19 @@
         <v>66</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D14" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="F14" s="30" t="s">
         <v>109</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>110</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="37"/>
@@ -1813,29 +1813,29 @@
         <v>66</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D15" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="F15" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>111</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>112</v>
       </c>
       <c r="H15" s="37">
         <v>5</v>
       </c>
       <c r="I15" s="37"/>
       <c r="J15" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K15" s="45" t="s">
         <v>69</v>
@@ -1847,7 +1847,7 @@
         <v>43</v>
       </c>
       <c r="N15" s="47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O15" s="44" t="s">
         <v>19</v>
@@ -1863,29 +1863,29 @@
         <v>66</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="G16" s="36" t="s">
         <v>115</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>116</v>
       </c>
       <c r="H16" s="37">
         <v>6</v>
       </c>
       <c r="I16" s="37"/>
       <c r="J16" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K16" s="45" t="s">
         <v>69</v>
@@ -1897,7 +1897,7 @@
         <v>44</v>
       </c>
       <c r="N16" s="47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O16" s="44" t="s">
         <v>19</v>
@@ -1913,29 +1913,29 @@
         <v>66</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="G17" s="36" t="s">
         <v>119</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>120</v>
       </c>
       <c r="H17" s="37">
         <v>7</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" s="45" t="s">
         <v>69</v>
@@ -1947,7 +1947,7 @@
         <v>85</v>
       </c>
       <c r="N17" s="47" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O17" s="44" t="s">
         <v>19</v>
@@ -1963,19 +1963,19 @@
         <v>66</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="36"/>
       <c r="H18" s="37"/>
@@ -1997,19 +1997,19 @@
         <v>66</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G19" s="36"/>
       <c r="H19" s="37"/>
@@ -2031,19 +2031,19 @@
         <v>66</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="37"/>
@@ -2065,27 +2065,27 @@
         <v>66</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="36" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="H21" s="37">
         <v>8</v>
       </c>
       <c r="I21" s="37"/>
       <c r="J21" s="38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K21" s="45" t="s">
         <v>69</v>
@@ -2111,25 +2111,25 @@
         <v>66</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="30"/>
       <c r="G22" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H22" s="37">
         <v>9</v>
       </c>
       <c r="I22" s="37"/>
       <c r="J22" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K22" s="45" t="s">
         <v>69</v>
@@ -2157,21 +2157,21 @@
         <v>87</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H23" s="37">
         <v>10</v>
       </c>
       <c r="I23" s="37"/>
       <c r="J23" s="38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K23" s="45" t="s">
         <v>69</v>
@@ -2199,10 +2199,10 @@
         <v>87</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="36"/>
@@ -2227,21 +2227,21 @@
         <v>87</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H25" s="37">
         <v>11</v>
       </c>
       <c r="I25" s="37"/>
       <c r="J25" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K25" s="45" t="s">
         <v>69</v>
@@ -2269,19 +2269,19 @@
         <v>87</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="30"/>
       <c r="G26" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H26" s="37">
         <v>12</v>
       </c>
       <c r="I26" s="37"/>
       <c r="J26" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K26" s="45" t="s">
         <v>70</v>
@@ -2295,19 +2295,19 @@
         <v>19</v>
       </c>
       <c r="P26" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q26" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="R26" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="Q26" s="51" t="s">
+      <c r="S26" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="T26" s="51" t="s">
         <v>159</v>
-      </c>
-      <c r="R26" s="51" t="s">
-        <v>160</v>
-      </c>
-      <c r="S26" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="T26" s="51" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -2317,19 +2317,19 @@
         <v>87</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="30"/>
       <c r="G27" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H27" s="37">
         <v>13</v>
       </c>
       <c r="I27" s="37"/>
       <c r="J27" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K27" s="45" t="s">
         <v>69</v>
@@ -2341,7 +2341,7 @@
         <v>43</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O27" s="44" t="s">
         <v>19</v>
@@ -2359,21 +2359,21 @@
         <v>87</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H28" s="37">
         <v>14</v>
       </c>
       <c r="I28" s="37"/>
       <c r="J28" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K28" s="45" t="s">
         <v>69</v>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="M28" s="46"/>
       <c r="N28" s="52" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O28" s="44" t="s">
         <v>19</v>
@@ -2401,19 +2401,19 @@
         <v>87</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="30"/>
       <c r="G29" s="40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H29" s="37">
         <v>15</v>
       </c>
       <c r="I29" s="37"/>
       <c r="J29" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K29" s="45" t="s">
         <v>69</v>
@@ -2441,19 +2441,19 @@
         <v>87</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" s="29"/>
       <c r="F30" s="30"/>
       <c r="G30" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H30" s="37">
         <v>16</v>
       </c>
       <c r="I30" s="37"/>
       <c r="J30" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K30" s="45" t="s">
         <v>69</v>
@@ -2480,14 +2480,14 @@
       <c r="E31" s="29"/>
       <c r="F31" s="30"/>
       <c r="G31" s="36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H31" s="37">
         <v>17</v>
       </c>
       <c r="I31" s="37"/>
       <c r="J31" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K31" s="45" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
ajustes según criterios nuevos.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="178">
   <si>
     <t>Asignatura</t>
   </si>
@@ -286,21 +286,9 @@
     <t>Regímenes políticos en América Latina</t>
   </si>
   <si>
-    <t>La Revolución Mexicana</t>
-  </si>
-  <si>
-    <t>Causas de la Revolución</t>
-  </si>
-  <si>
     <t>El desarrollo de la Revolución</t>
   </si>
   <si>
-    <t>Sublevaciones en el norte</t>
-  </si>
-  <si>
-    <t>Sublevaciones en el sur</t>
-  </si>
-  <si>
     <t xml:space="preserve">El triunfo de Madero </t>
   </si>
   <si>
@@ -310,18 +298,9 @@
     <t>La intervención de Estados Unidos</t>
   </si>
   <si>
-    <t>Guerra entre líderes</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Conoce los detalles de la Expedición Punitiva</t>
-  </si>
-  <si>
     <t>Actividad que permite conocer detalles de la Expedición Punitiva que Estados Unidos adelantó contra Pancho Villa</t>
   </si>
   <si>
-    <t>Presidencia de Venustiano Carranza</t>
-  </si>
-  <si>
     <t>Las presidencias de Obregón y Calles</t>
   </si>
   <si>
@@ -337,9 +316,6 @@
     <t>Consolidación</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La Revolución Mexicana</t>
-  </si>
-  <si>
     <t>Interactivo con video que relata aspectos generales de la Revolución Mexicana</t>
   </si>
   <si>
@@ -379,9 +355,6 @@
     <t xml:space="preserve">Perú </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: El pensamiento de Víctor Raúl Haya de la Torre</t>
-  </si>
-  <si>
     <t>Actividad que permite conocer los principios que sustentaron el populismo desde el pensamiento de su principal ideólogo: Víctor Raúl Haya de la Torre</t>
   </si>
   <si>
@@ -400,27 +373,18 @@
     <t>Dictaduras militares</t>
   </si>
   <si>
-    <t>Practica: Las dictaduras militares</t>
-  </si>
-  <si>
     <t>Actividad que permite revisar en dónde y cuándo ocurrieron dictaduras militares de América Latina</t>
   </si>
   <si>
     <t>Encuentra nombres de líderes y términos relacionados con el populismo y las dictaduras militares</t>
   </si>
   <si>
-    <t>Sopa de letras para encontrar nombres y términos relacionados con el populismo y las dictaduras militares</t>
-  </si>
-  <si>
     <t>El desarrollo industrial de América Latina</t>
   </si>
   <si>
     <t>Industrialización por sustitución de importaciones</t>
   </si>
   <si>
-    <t>Practica: La industrialización por sustitución de importaciones</t>
-  </si>
-  <si>
     <t>Interactivo para repasar aspectos generales de la industrialización por sustitución de importaciones</t>
   </si>
   <si>
@@ -436,18 +400,9 @@
     <t>Interactivo con audio que permite conocer el concepto de ciudades resilientes</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Descubre la relación que existe entre pobreza y urbanización</t>
-  </si>
-  <si>
-    <t>Ejercicio que permite para constatar cómo se transformaron los niveles de pobreza urbana y rural desde los años setenta en adelante</t>
-  </si>
-  <si>
     <t>Competencias</t>
   </si>
   <si>
-    <t>Competencias: Regímenes políticos en América Latina</t>
-  </si>
-  <si>
     <t>Actividad para agrupar características generales de regímenes políticos que vivió América Latina</t>
   </si>
   <si>
@@ -460,13 +415,7 @@
     <t>Mapa conceptual que sintetiza aspectos políticos de América Latina</t>
   </si>
   <si>
-    <t>Actividad que sintetiza aspectos generales de la vida política y económica de América Latina</t>
-  </si>
-  <si>
     <t>CS_09_03_CO</t>
-  </si>
-  <si>
-    <t>M101</t>
   </si>
   <si>
     <t>Actividad con  fragmentos de texto</t>
@@ -524,13 +473,106 @@
     <t>Actividad con audio. Se indica páginas para descargarlo.</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>El Plan Ayala</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: El populismo en América Latina</t>
+  </si>
+  <si>
+    <t>Profundiza: Mexico en el siglo XIX</t>
+  </si>
+  <si>
+    <t>Las causas de la Revolución</t>
+  </si>
+  <si>
+    <t>La guerra entre líderes</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La Revolución mexicana</t>
+  </si>
+  <si>
+    <t>Las sublevaciones en el norte</t>
+  </si>
+  <si>
+    <t>Las sublevaciones en el sur</t>
+  </si>
+  <si>
+    <t>La presidencia de Venustiano Carranza</t>
+  </si>
+  <si>
+    <t>Actividad para identificar nombres y términos relacionados con el populismo y las dictaduras militares</t>
+  </si>
+  <si>
+    <t>Conoce cómo era México en el siglo XIX en el aspecto social y político</t>
+  </si>
+  <si>
+    <t>La Revolución mexicana</t>
+  </si>
+  <si>
+    <t>La Revolucion mexicana</t>
+  </si>
+  <si>
+    <t>Conoce los detalles de la Expedición Punitiva</t>
+  </si>
+  <si>
+    <t>El pensamiento de Víctor Raúl Haya de la Torre</t>
+  </si>
+  <si>
+    <t>Las dictaduras militares</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las dictaduras militares</t>
+  </si>
+  <si>
+    <t>La industrialización por sustitución de importaciones</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El desarrollo industrial de América Latina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los problemas de la ciudad</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El desarrollo urbano del continente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: Actividad que ayuda a comprender y recordar los principales aspectos de los regímenes políticas de América Latina  </t>
+  </si>
+  <si>
+    <t>Competencias: Actividad para fortalecer conceptos y procesos relacionados con los regímenes de América Latina</t>
+  </si>
+  <si>
+    <t>Actividad sobre La Revolución mexicana ESTA LISTO EL MOTOR PERO DEBEN COMPLETARSE LAS 10 PREGUNTAS</t>
+  </si>
+  <si>
+    <t>Actividad sobre El populismo en América Latina. Esta listo el motor pero hay que completar las diez preguntas.</t>
+  </si>
+  <si>
+    <t>Actividad sobre Las dictaduras militares. Está listo el motor pero falta completar las 10 preguntas.</t>
+  </si>
+  <si>
+    <t>Actividad sobre El desarrollo industrial de América Latina. ESTA LISTO EL MOTOR PERO DEBEN COMPLETARSE LAS 10 PREGUNTAS</t>
+  </si>
+  <si>
+    <t>Actividad sobre El desarrollo urbano del continente.ESTA LISTO EL MOTOR PERO DEBEN COMPLETARSE LAS 10 PREGUNTAS</t>
+  </si>
+  <si>
+    <t>Grandes cambios políticos en América Latina</t>
+  </si>
+  <si>
+    <t>Actividad para revisar algunos hechos de América Latina</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos sobre Los regímenes políticos en América Latina</t>
   </si>
 </sst>
 </file>
@@ -573,7 +615,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +661,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -907,7 +955,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,8 +978,44 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1214,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,181 +1392,183 @@
         <v>66</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="33"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="35"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="44"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
       <c r="S2" s="14"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="1:20" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F3" s="53"/>
+      <c r="G3" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="55">
+        <v>1</v>
+      </c>
+      <c r="I3" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="K3" s="52"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="61"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="F4" s="30" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
       <c r="J4" s="38"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="43"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="F5" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" s="37">
-        <v>1</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="K5" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="N5" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="O5" s="44" t="s">
-        <v>19</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="43"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="F6" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="44"/>
+        <v>89</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" s="37">
+        <v>2</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
@@ -1495,183 +1580,183 @@
         <v>66</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D7" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>90</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>95</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="38"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="43"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="37">
-        <v>2</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="K8" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F8" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="2"/>
+      <c r="F9" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="37">
+        <v>3</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="O9" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="4"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D10" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="F10" s="30" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="37"/>
       <c r="I10" s="37"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="44"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="43"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="F11" s="30" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="37"/>
       <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="44"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="43"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
@@ -1683,89 +1768,79 @@
         <v>66</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D12" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="37">
-        <v>3</v>
-      </c>
+      <c r="F12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N12" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="J12" s="38"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="43"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
       <c r="S12" s="13"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D13" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="30"/>
+      <c r="F13" s="30" t="s">
+        <v>94</v>
+      </c>
       <c r="G13" s="36" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H13" s="37">
         <v>4</v>
       </c>
-      <c r="I13" s="37"/>
+      <c r="I13" s="37" t="s">
+        <v>19</v>
+      </c>
       <c r="J13" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="K13" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="K13" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="O13" s="44" t="s">
+      <c r="L13" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="O13" s="43" t="s">
         <v>19</v>
       </c>
       <c r="P13" s="1"/>
@@ -1774,34 +1849,42 @@
       <c r="S13" s="13"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>107</v>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+        <v>95</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="37">
+        <v>5</v>
+      </c>
       <c r="I14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="44"/>
+      <c r="J14" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="N14" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
@@ -1813,95 +1896,73 @@
         <v>66</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="37">
-        <v>5</v>
-      </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="K15" s="45" t="s">
+      <c r="D15" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="63"/>
+      <c r="G15" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="65">
+        <v>6</v>
+      </c>
+      <c r="I15" s="65"/>
+      <c r="J15" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K15" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="46" t="s">
+      <c r="L15" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N15" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="O15" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="M15" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="69"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="72"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" s="37">
-        <v>6</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="37"/>
-      <c r="J16" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="K16" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="N16" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="O16" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="J16" s="38"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="43"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
@@ -1913,43 +1974,43 @@
         <v>66</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="H17" s="37">
         <v>7</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="K17" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="46" t="s">
+      <c r="L17" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="N17" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="O17" s="44" t="s">
+      <c r="M17" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="O17" s="43" t="s">
         <v>19</v>
       </c>
       <c r="P17" s="1"/>
@@ -1958,68 +2019,100 @@
       <c r="S17" s="13"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="H18" s="37">
+        <v>8</v>
+      </c>
       <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="44"/>
+      <c r="J18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="O18" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
       <c r="S18" s="13"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+        <v>110</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="37">
+        <v>9</v>
+      </c>
       <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="44"/>
+      <c r="J19" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="N19" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="O19" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
@@ -2031,29 +2124,29 @@
         <v>66</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
       <c r="J20" s="38"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="43"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
@@ -2065,41 +2158,29 @@
         <v>66</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="H21" s="37">
-        <v>8</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="37"/>
-      <c r="J21" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="K21" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="N21" s="47"/>
-      <c r="O21" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="J21" s="38"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="43"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
@@ -2111,79 +2192,75 @@
         <v>66</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" s="37">
-        <v>9</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="37"/>
-      <c r="J22" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="K22" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="N22" s="47"/>
-      <c r="O22" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="J22" s="38"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="43"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
       <c r="S22" s="13"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>131</v>
+      </c>
       <c r="C23" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="30"/>
+        <v>109</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>114</v>
+      </c>
       <c r="G23" s="36" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="H23" s="37">
         <v>10</v>
       </c>
       <c r="I23" s="37"/>
       <c r="J23" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="K23" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="47"/>
-      <c r="O23" s="44" t="s">
+      <c r="M23" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="N23" s="46"/>
+      <c r="O23" s="43" t="s">
         <v>19</v>
       </c>
       <c r="P23" s="1"/>
@@ -2192,68 +2269,80 @@
       <c r="S23" s="13"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="21" t="s">
+    <row r="24" spans="1:20" s="62" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="29" t="s">
+      <c r="D24" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24" s="65">
+        <v>11</v>
+      </c>
+      <c r="I24" s="65"/>
+      <c r="J24" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="K24" s="67"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="71"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="72"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="2"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
       <c r="C25" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>104</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E25" s="29"/>
       <c r="F25" s="30"/>
       <c r="G25" s="36" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="H25" s="37">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I25" s="37"/>
       <c r="J25" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="K25" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="46" t="s">
+      <c r="L25" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="47"/>
-      <c r="O25" s="44" t="s">
+      <c r="M25" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="N25" s="46"/>
+      <c r="O25" s="43" t="s">
         <v>19</v>
       </c>
       <c r="P25" s="1"/>
@@ -2262,132 +2351,100 @@
       <c r="S25" s="13"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="21" t="s">
-        <v>87</v>
-      </c>
+    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="26" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="30"/>
       <c r="G26" s="36" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="H26" s="37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I26" s="37"/>
       <c r="J26" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="K26" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M26" s="46"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="K26" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="46"/>
+      <c r="O26" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="P26" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q26" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="R26" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="S26" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="T26" s="51" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="21" t="s">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="H27" s="37">
-        <v>13</v>
-      </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="K27" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L27" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M27" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N27" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="O27" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="2"/>
-    </row>
-    <row r="28" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="D27" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" s="65">
+        <v>14</v>
+      </c>
+      <c r="I27" s="65"/>
+      <c r="J27" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="K27" s="67"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="71"/>
+      <c r="R27" s="71"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="72"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="21" t="s">
         <v>87</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F28" s="30"/>
-      <c r="G28" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="H28" s="37">
-        <v>14</v>
-      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="37"/>
-      <c r="J28" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="K28" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M28" s="46"/>
-      <c r="N28" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="O28" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="J28" s="38"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="43"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
@@ -2401,31 +2458,33 @@
         <v>87</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="E29" s="29"/>
+        <v>119</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>160</v>
+      </c>
       <c r="F29" s="30"/>
-      <c r="G29" s="40" t="s">
-        <v>141</v>
+      <c r="G29" s="36" t="s">
+        <v>162</v>
       </c>
       <c r="H29" s="37">
         <v>15</v>
       </c>
       <c r="I29" s="37"/>
       <c r="J29" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="K29" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="K29" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L29" s="46" t="s">
+      <c r="L29" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="N29" s="47"/>
-      <c r="O29" s="44" t="s">
+      <c r="M29" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" s="46"/>
+      <c r="O29" s="43" t="s">
         <v>19</v>
       </c>
       <c r="P29" s="1"/>
@@ -2434,96 +2493,122 @@
       <c r="S29" s="13"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="H30" s="37">
+    <row r="30" spans="1:20" s="62" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="73"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="65">
         <v>16</v>
       </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="K30" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="46"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="2"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="K30" s="67"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="70"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="71"/>
+      <c r="T30" s="73"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="C31" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="E31" s="29"/>
       <c r="F31" s="30"/>
       <c r="G31" s="36" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H31" s="37">
         <v>17</v>
       </c>
       <c r="I31" s="37"/>
       <c r="J31" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="K31" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="M31" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="N31" s="47"/>
-      <c r="O31" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" s="45"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="2"/>
+      <c r="P31" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q31" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="R31" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="S31" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="T31" s="50" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="C32" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="44"/>
+      <c r="G32" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="37">
+        <v>18</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="K32" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="N32" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="O32" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
@@ -2533,19 +2618,35 @@
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="C33" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="E33" s="29"/>
       <c r="F33" s="30"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="G33" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="37">
+        <v>19</v>
+      </c>
       <c r="I33" s="37"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="44"/>
+      <c r="J33" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="K33" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="M33" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" s="46"/>
+      <c r="O33" s="43"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
@@ -2555,107 +2656,163 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="26"/>
       <c r="E34" s="29"/>
       <c r="F34" s="30"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
+      <c r="G34" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="37">
+        <v>20</v>
+      </c>
       <c r="I34" s="37"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="44"/>
+      <c r="J34" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="K34" s="44"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="49"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
-      <c r="T34" s="2"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="44"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="2"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="2"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="47"/>
-      <c r="O37" s="44"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="2"/>
+      <c r="T34" s="74"/>
+    </row>
+    <row r="35" spans="1:20" s="62" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="73"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="63"/>
+      <c r="G35" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="65">
+        <v>21</v>
+      </c>
+      <c r="I35" s="65"/>
+      <c r="J35" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="K35" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="M35" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="69"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="70"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="71"/>
+      <c r="T35" s="73"/>
+    </row>
+    <row r="36" spans="1:20" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="73"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="67"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="H36" s="65">
+        <v>22</v>
+      </c>
+      <c r="I36" s="65"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="69"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="70"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="71"/>
+      <c r="S36" s="71"/>
+      <c r="T36" s="73"/>
+    </row>
+    <row r="37" spans="1:20" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="73"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="67"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="H37" s="65">
+        <v>23</v>
+      </c>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="70"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="73"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
+      <c r="C38" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>128</v>
+      </c>
       <c r="E38" s="29"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
+      <c r="G38" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="H38" s="37">
+        <v>24</v>
+      </c>
       <c r="I38" s="37"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="44"/>
+      <c r="J38" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="K38" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="45"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
@@ -2669,15 +2826,29 @@
       <c r="D39" s="26"/>
       <c r="E39" s="29"/>
       <c r="F39" s="30"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
+      <c r="G39" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="H39" s="37">
+        <v>25</v>
+      </c>
       <c r="I39" s="37"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="46"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="44"/>
+      <c r="J39" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="M39" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="N39" s="46"/>
+      <c r="O39" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
@@ -2695,18 +2866,18 @@
       <c r="H40" s="37"/>
       <c r="I40" s="37"/>
       <c r="J40" s="38"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="43"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
@@ -2717,11 +2888,11 @@
       <c r="H41" s="37"/>
       <c r="I41" s="37"/>
       <c r="J41" s="38"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="46"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="43"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
@@ -2739,11 +2910,11 @@
       <c r="H42" s="37"/>
       <c r="I42" s="37"/>
       <c r="J42" s="38"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
-      <c r="N42" s="47"/>
-      <c r="O42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="43"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
@@ -2760,12 +2931,12 @@
       <c r="G43" s="36"/>
       <c r="H43" s="37"/>
       <c r="I43" s="37"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="46"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="44"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="43"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
@@ -2783,11 +2954,11 @@
       <c r="H44" s="37"/>
       <c r="I44" s="37"/>
       <c r="J44" s="38"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="46"/>
-      <c r="N44" s="47"/>
-      <c r="O44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
+      <c r="N44" s="46"/>
+      <c r="O44" s="43"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
@@ -2798,18 +2969,18 @@
       <c r="A45" s="23"/>
       <c r="B45" s="24"/>
       <c r="C45" s="25"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
       <c r="G45" s="36"/>
       <c r="H45" s="37"/>
       <c r="I45" s="37"/>
       <c r="J45" s="38"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="47"/>
-      <c r="O45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="43"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="13"/>
       <c r="R45" s="13"/>
@@ -2820,18 +2991,18 @@
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="30"/>
       <c r="G46" s="36"/>
       <c r="H46" s="37"/>
       <c r="I46" s="37"/>
       <c r="J46" s="38"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="46"/>
+      <c r="O46" s="43"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="13"/>
       <c r="R46" s="13"/>
@@ -2842,18 +3013,18 @@
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="25"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="32"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="30"/>
       <c r="G47" s="36"/>
       <c r="H47" s="37"/>
       <c r="I47" s="37"/>
       <c r="J47" s="38"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="47"/>
-      <c r="O47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="45"/>
+      <c r="M47" s="45"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="43"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="13"/>
       <c r="R47" s="13"/>
@@ -2864,40 +3035,40 @@
       <c r="A48" s="23"/>
       <c r="B48" s="24"/>
       <c r="C48" s="25"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="30"/>
       <c r="G48" s="36"/>
       <c r="H48" s="37"/>
       <c r="I48" s="37"/>
       <c r="J48" s="38"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="47"/>
-      <c r="O48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="45"/>
+      <c r="M48" s="45"/>
+      <c r="N48" s="46"/>
+      <c r="O48" s="43"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
       <c r="S48" s="13"/>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="24"/>
       <c r="C49" s="25"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="30"/>
       <c r="G49" s="36"/>
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="38"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="46"/>
-      <c r="N49" s="47"/>
-      <c r="O49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="46"/>
+      <c r="O49" s="43"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="13"/>
       <c r="R49" s="13"/>
@@ -2908,18 +3079,18 @@
       <c r="A50" s="23"/>
       <c r="B50" s="24"/>
       <c r="C50" s="25"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
       <c r="G50" s="36"/>
       <c r="H50" s="37"/>
       <c r="I50" s="37"/>
       <c r="J50" s="38"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="46"/>
-      <c r="M50" s="46"/>
-      <c r="N50" s="47"/>
-      <c r="O50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="43"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="13"/>
       <c r="R50" s="13"/>
@@ -2930,18 +3101,18 @@
       <c r="A51" s="23"/>
       <c r="B51" s="24"/>
       <c r="C51" s="25"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="36"/>
       <c r="H51" s="37"/>
       <c r="I51" s="37"/>
       <c r="J51" s="38"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="46"/>
-      <c r="M51" s="46"/>
-      <c r="N51" s="47"/>
-      <c r="O51" s="44"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="46"/>
+      <c r="O51" s="43"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="13"/>
       <c r="R51" s="13"/>
@@ -2952,18 +3123,18 @@
       <c r="A52" s="23"/>
       <c r="B52" s="24"/>
       <c r="C52" s="25"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="30"/>
       <c r="G52" s="36"/>
       <c r="H52" s="37"/>
       <c r="I52" s="37"/>
       <c r="J52" s="38"/>
-      <c r="K52" s="45"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="46"/>
+      <c r="O52" s="43"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="13"/>
       <c r="R52" s="13"/>
@@ -2981,11 +3152,11 @@
       <c r="H53" s="37"/>
       <c r="I53" s="37"/>
       <c r="J53" s="38"/>
-      <c r="K53" s="45"/>
-      <c r="L53" s="46"/>
-      <c r="M53" s="46"/>
-      <c r="N53" s="47"/>
-      <c r="O53" s="44"/>
+      <c r="K53" s="44"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="45"/>
+      <c r="N53" s="46"/>
+      <c r="O53" s="43"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="13"/>
       <c r="R53" s="13"/>
@@ -3003,11 +3174,11 @@
       <c r="H54" s="37"/>
       <c r="I54" s="37"/>
       <c r="J54" s="38"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="47"/>
-      <c r="O54" s="44"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="46"/>
+      <c r="O54" s="43"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="13"/>
       <c r="R54" s="13"/>
@@ -3025,11 +3196,11 @@
       <c r="H55" s="37"/>
       <c r="I55" s="37"/>
       <c r="J55" s="38"/>
-      <c r="K55" s="45"/>
-      <c r="L55" s="46"/>
-      <c r="M55" s="46"/>
-      <c r="N55" s="47"/>
-      <c r="O55" s="44"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="45"/>
+      <c r="N55" s="46"/>
+      <c r="O55" s="43"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="13"/>
       <c r="R55" s="13"/>
@@ -3047,11 +3218,11 @@
       <c r="H56" s="37"/>
       <c r="I56" s="37"/>
       <c r="J56" s="38"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="47"/>
-      <c r="O56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="45"/>
+      <c r="M56" s="45"/>
+      <c r="N56" s="46"/>
+      <c r="O56" s="43"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="13"/>
       <c r="R56" s="13"/>
@@ -3069,11 +3240,11 @@
       <c r="H57" s="37"/>
       <c r="I57" s="37"/>
       <c r="J57" s="38"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="46"/>
-      <c r="M57" s="46"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="44"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="45"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="46"/>
+      <c r="O57" s="43"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="13"/>
       <c r="R57" s="13"/>
@@ -3091,11 +3262,11 @@
       <c r="H58" s="37"/>
       <c r="I58" s="37"/>
       <c r="J58" s="38"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="47"/>
-      <c r="O58" s="44"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="46"/>
+      <c r="O58" s="43"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="13"/>
       <c r="R58" s="13"/>
@@ -3113,11 +3284,11 @@
       <c r="H59" s="37"/>
       <c r="I59" s="37"/>
       <c r="J59" s="38"/>
-      <c r="K59" s="45"/>
-      <c r="L59" s="46"/>
-      <c r="M59" s="46"/>
-      <c r="N59" s="47"/>
-      <c r="O59" s="44"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="45"/>
+      <c r="M59" s="45"/>
+      <c r="N59" s="46"/>
+      <c r="O59" s="43"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
@@ -3135,11 +3306,11 @@
       <c r="H60" s="37"/>
       <c r="I60" s="37"/>
       <c r="J60" s="38"/>
-      <c r="K60" s="45"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="46"/>
-      <c r="N60" s="47"/>
-      <c r="O60" s="44"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="45"/>
+      <c r="M60" s="45"/>
+      <c r="N60" s="46"/>
+      <c r="O60" s="43"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
@@ -3157,11 +3328,11 @@
       <c r="H61" s="37"/>
       <c r="I61" s="37"/>
       <c r="J61" s="38"/>
-      <c r="K61" s="45"/>
-      <c r="L61" s="46"/>
-      <c r="M61" s="46"/>
-      <c r="N61" s="47"/>
-      <c r="O61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="45"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="46"/>
+      <c r="O61" s="43"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="13"/>
       <c r="R61" s="13"/>
@@ -3179,11 +3350,11 @@
       <c r="H62" s="37"/>
       <c r="I62" s="37"/>
       <c r="J62" s="38"/>
-      <c r="K62" s="45"/>
-      <c r="L62" s="46"/>
-      <c r="M62" s="46"/>
-      <c r="N62" s="47"/>
-      <c r="O62" s="44"/>
+      <c r="K62" s="44"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="46"/>
+      <c r="O62" s="43"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="13"/>
       <c r="R62" s="13"/>
@@ -3201,11 +3372,11 @@
       <c r="H63" s="37"/>
       <c r="I63" s="37"/>
       <c r="J63" s="38"/>
-      <c r="K63" s="45"/>
-      <c r="L63" s="46"/>
-      <c r="M63" s="46"/>
-      <c r="N63" s="47"/>
-      <c r="O63" s="44"/>
+      <c r="K63" s="44"/>
+      <c r="L63" s="45"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="46"/>
+      <c r="O63" s="43"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="13"/>
       <c r="R63" s="13"/>
@@ -3223,11 +3394,11 @@
       <c r="H64" s="37"/>
       <c r="I64" s="37"/>
       <c r="J64" s="38"/>
-      <c r="K64" s="45"/>
-      <c r="L64" s="46"/>
-      <c r="M64" s="46"/>
-      <c r="N64" s="47"/>
-      <c r="O64" s="44"/>
+      <c r="K64" s="44"/>
+      <c r="L64" s="45"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="46"/>
+      <c r="O64" s="43"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="13"/>
       <c r="R64" s="13"/>
@@ -3245,11 +3416,11 @@
       <c r="H65" s="37"/>
       <c r="I65" s="37"/>
       <c r="J65" s="38"/>
-      <c r="K65" s="45"/>
-      <c r="L65" s="46"/>
-      <c r="M65" s="46"/>
-      <c r="N65" s="47"/>
-      <c r="O65" s="44"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="46"/>
+      <c r="O65" s="43"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="13"/>
       <c r="R65" s="13"/>
@@ -3267,11 +3438,11 @@
       <c r="H66" s="37"/>
       <c r="I66" s="37"/>
       <c r="J66" s="38"/>
-      <c r="K66" s="45"/>
-      <c r="L66" s="46"/>
-      <c r="M66" s="46"/>
-      <c r="N66" s="47"/>
-      <c r="O66" s="44"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="45"/>
+      <c r="M66" s="45"/>
+      <c r="N66" s="46"/>
+      <c r="O66" s="43"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="13"/>
       <c r="R66" s="13"/>
@@ -3289,11 +3460,11 @@
       <c r="H67" s="37"/>
       <c r="I67" s="37"/>
       <c r="J67" s="38"/>
-      <c r="K67" s="45"/>
-      <c r="L67" s="46"/>
-      <c r="M67" s="46"/>
-      <c r="N67" s="47"/>
-      <c r="O67" s="44"/>
+      <c r="K67" s="44"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="46"/>
+      <c r="O67" s="43"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="13"/>
       <c r="R67" s="13"/>
@@ -3311,11 +3482,11 @@
       <c r="H68" s="37"/>
       <c r="I68" s="37"/>
       <c r="J68" s="38"/>
-      <c r="K68" s="45"/>
-      <c r="L68" s="46"/>
-      <c r="M68" s="46"/>
-      <c r="N68" s="47"/>
-      <c r="O68" s="44"/>
+      <c r="K68" s="44"/>
+      <c r="L68" s="45"/>
+      <c r="M68" s="45"/>
+      <c r="N68" s="46"/>
+      <c r="O68" s="43"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="13"/>
       <c r="R68" s="13"/>
@@ -3333,11 +3504,11 @@
       <c r="H69" s="37"/>
       <c r="I69" s="37"/>
       <c r="J69" s="38"/>
-      <c r="K69" s="45"/>
-      <c r="L69" s="46"/>
-      <c r="M69" s="46"/>
-      <c r="N69" s="47"/>
-      <c r="O69" s="44"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="45"/>
+      <c r="M69" s="45"/>
+      <c r="N69" s="46"/>
+      <c r="O69" s="43"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="13"/>
       <c r="R69" s="13"/>
@@ -3355,11 +3526,11 @@
       <c r="H70" s="37"/>
       <c r="I70" s="37"/>
       <c r="J70" s="38"/>
-      <c r="K70" s="45"/>
-      <c r="L70" s="46"/>
-      <c r="M70" s="46"/>
-      <c r="N70" s="47"/>
-      <c r="O70" s="44"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="45"/>
+      <c r="M70" s="45"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="43"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="13"/>
       <c r="R70" s="13"/>
@@ -3377,11 +3548,11 @@
       <c r="H71" s="37"/>
       <c r="I71" s="37"/>
       <c r="J71" s="38"/>
-      <c r="K71" s="45"/>
-      <c r="L71" s="46"/>
-      <c r="M71" s="46"/>
-      <c r="N71" s="47"/>
-      <c r="O71" s="44"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="45"/>
+      <c r="M71" s="45"/>
+      <c r="N71" s="46"/>
+      <c r="O71" s="43"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="13"/>
       <c r="R71" s="13"/>
@@ -3399,11 +3570,11 @@
       <c r="H72" s="37"/>
       <c r="I72" s="37"/>
       <c r="J72" s="38"/>
-      <c r="K72" s="45"/>
-      <c r="L72" s="46"/>
-      <c r="M72" s="46"/>
-      <c r="N72" s="47"/>
-      <c r="O72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="45"/>
+      <c r="M72" s="45"/>
+      <c r="N72" s="46"/>
+      <c r="O72" s="43"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="13"/>
       <c r="R72" s="13"/>
@@ -3421,11 +3592,11 @@
       <c r="H73" s="37"/>
       <c r="I73" s="37"/>
       <c r="J73" s="38"/>
-      <c r="K73" s="45"/>
-      <c r="L73" s="46"/>
-      <c r="M73" s="46"/>
-      <c r="N73" s="47"/>
-      <c r="O73" s="44"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="45"/>
+      <c r="M73" s="45"/>
+      <c r="N73" s="46"/>
+      <c r="O73" s="43"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="13"/>
       <c r="R73" s="13"/>
@@ -3443,11 +3614,11 @@
       <c r="H74" s="37"/>
       <c r="I74" s="37"/>
       <c r="J74" s="38"/>
-      <c r="K74" s="45"/>
-      <c r="L74" s="46"/>
-      <c r="M74" s="46"/>
-      <c r="N74" s="47"/>
-      <c r="O74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="45"/>
+      <c r="M74" s="45"/>
+      <c r="N74" s="46"/>
+      <c r="O74" s="43"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="13"/>
       <c r="R74" s="13"/>
@@ -3465,11 +3636,11 @@
       <c r="H75" s="37"/>
       <c r="I75" s="37"/>
       <c r="J75" s="38"/>
-      <c r="K75" s="45"/>
-      <c r="L75" s="46"/>
-      <c r="M75" s="46"/>
-      <c r="N75" s="47"/>
-      <c r="O75" s="44"/>
+      <c r="K75" s="44"/>
+      <c r="L75" s="45"/>
+      <c r="M75" s="45"/>
+      <c r="N75" s="46"/>
+      <c r="O75" s="43"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="13"/>
       <c r="R75" s="13"/>
@@ -3487,11 +3658,11 @@
       <c r="H76" s="37"/>
       <c r="I76" s="37"/>
       <c r="J76" s="38"/>
-      <c r="K76" s="45"/>
-      <c r="L76" s="46"/>
-      <c r="M76" s="46"/>
-      <c r="N76" s="47"/>
-      <c r="O76" s="44"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="45"/>
+      <c r="M76" s="45"/>
+      <c r="N76" s="46"/>
+      <c r="O76" s="43"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="13"/>
       <c r="R76" s="13"/>
@@ -3509,11 +3680,11 @@
       <c r="H77" s="37"/>
       <c r="I77" s="37"/>
       <c r="J77" s="38"/>
-      <c r="K77" s="45"/>
-      <c r="L77" s="46"/>
-      <c r="M77" s="46"/>
-      <c r="N77" s="47"/>
-      <c r="O77" s="44"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="45"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="46"/>
+      <c r="O77" s="43"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="13"/>
       <c r="R77" s="13"/>
@@ -3531,11 +3702,11 @@
       <c r="H78" s="37"/>
       <c r="I78" s="37"/>
       <c r="J78" s="38"/>
-      <c r="K78" s="45"/>
-      <c r="L78" s="46"/>
-      <c r="M78" s="46"/>
-      <c r="N78" s="47"/>
-      <c r="O78" s="44"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="45"/>
+      <c r="M78" s="45"/>
+      <c r="N78" s="46"/>
+      <c r="O78" s="43"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
@@ -3553,11 +3724,11 @@
       <c r="H79" s="37"/>
       <c r="I79" s="37"/>
       <c r="J79" s="38"/>
-      <c r="K79" s="45"/>
-      <c r="L79" s="46"/>
-      <c r="M79" s="46"/>
-      <c r="N79" s="47"/>
-      <c r="O79" s="44"/>
+      <c r="K79" s="44"/>
+      <c r="L79" s="45"/>
+      <c r="M79" s="45"/>
+      <c r="N79" s="46"/>
+      <c r="O79" s="43"/>
       <c r="P79" s="1"/>
       <c r="Q79" s="13"/>
       <c r="R79" s="13"/>
@@ -3575,11 +3746,11 @@
       <c r="H80" s="37"/>
       <c r="I80" s="37"/>
       <c r="J80" s="38"/>
-      <c r="K80" s="45"/>
-      <c r="L80" s="46"/>
-      <c r="M80" s="46"/>
-      <c r="N80" s="47"/>
-      <c r="O80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="45"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="46"/>
+      <c r="O80" s="43"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="13"/>
       <c r="R80" s="13"/>
@@ -3597,11 +3768,11 @@
       <c r="H81" s="37"/>
       <c r="I81" s="37"/>
       <c r="J81" s="38"/>
-      <c r="K81" s="45"/>
-      <c r="L81" s="46"/>
-      <c r="M81" s="46"/>
-      <c r="N81" s="47"/>
-      <c r="O81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="45"/>
+      <c r="M81" s="45"/>
+      <c r="N81" s="46"/>
+      <c r="O81" s="43"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="13"/>
       <c r="R81" s="13"/>
@@ -3619,11 +3790,11 @@
       <c r="H82" s="37"/>
       <c r="I82" s="37"/>
       <c r="J82" s="38"/>
-      <c r="K82" s="45"/>
-      <c r="L82" s="46"/>
-      <c r="M82" s="46"/>
-      <c r="N82" s="47"/>
-      <c r="O82" s="44"/>
+      <c r="K82" s="44"/>
+      <c r="L82" s="45"/>
+      <c r="M82" s="45"/>
+      <c r="N82" s="46"/>
+      <c r="O82" s="43"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="13"/>
       <c r="R82" s="13"/>
@@ -3641,11 +3812,11 @@
       <c r="H83" s="37"/>
       <c r="I83" s="37"/>
       <c r="J83" s="38"/>
-      <c r="K83" s="45"/>
-      <c r="L83" s="46"/>
-      <c r="M83" s="46"/>
-      <c r="N83" s="47"/>
-      <c r="O83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="45"/>
+      <c r="M83" s="45"/>
+      <c r="N83" s="46"/>
+      <c r="O83" s="43"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="13"/>
       <c r="R83" s="13"/>
@@ -3663,11 +3834,11 @@
       <c r="H84" s="37"/>
       <c r="I84" s="37"/>
       <c r="J84" s="38"/>
-      <c r="K84" s="45"/>
-      <c r="L84" s="46"/>
-      <c r="M84" s="46"/>
-      <c r="N84" s="47"/>
-      <c r="O84" s="44"/>
+      <c r="K84" s="44"/>
+      <c r="L84" s="45"/>
+      <c r="M84" s="45"/>
+      <c r="N84" s="46"/>
+      <c r="O84" s="43"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="13"/>
       <c r="R84" s="13"/>
@@ -3685,11 +3856,11 @@
       <c r="H85" s="37"/>
       <c r="I85" s="37"/>
       <c r="J85" s="38"/>
-      <c r="K85" s="45"/>
-      <c r="L85" s="46"/>
-      <c r="M85" s="46"/>
-      <c r="N85" s="47"/>
-      <c r="O85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="45"/>
+      <c r="M85" s="45"/>
+      <c r="N85" s="46"/>
+      <c r="O85" s="43"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="13"/>
       <c r="R85" s="13"/>
@@ -3707,11 +3878,11 @@
       <c r="H86" s="37"/>
       <c r="I86" s="37"/>
       <c r="J86" s="38"/>
-      <c r="K86" s="45"/>
-      <c r="L86" s="46"/>
-      <c r="M86" s="46"/>
-      <c r="N86" s="47"/>
-      <c r="O86" s="44"/>
+      <c r="K86" s="44"/>
+      <c r="L86" s="45"/>
+      <c r="M86" s="45"/>
+      <c r="N86" s="46"/>
+      <c r="O86" s="43"/>
       <c r="P86" s="1"/>
       <c r="Q86" s="13"/>
       <c r="R86" s="13"/>
@@ -3729,11 +3900,11 @@
       <c r="H87" s="37"/>
       <c r="I87" s="37"/>
       <c r="J87" s="38"/>
-      <c r="K87" s="45"/>
-      <c r="L87" s="46"/>
-      <c r="M87" s="46"/>
-      <c r="N87" s="47"/>
-      <c r="O87" s="44"/>
+      <c r="K87" s="44"/>
+      <c r="L87" s="45"/>
+      <c r="M87" s="45"/>
+      <c r="N87" s="46"/>
+      <c r="O87" s="43"/>
       <c r="P87" s="1"/>
       <c r="Q87" s="13"/>
       <c r="R87" s="13"/>
@@ -3751,11 +3922,11 @@
       <c r="H88" s="37"/>
       <c r="I88" s="37"/>
       <c r="J88" s="38"/>
-      <c r="K88" s="45"/>
-      <c r="L88" s="46"/>
-      <c r="M88" s="46"/>
-      <c r="N88" s="47"/>
-      <c r="O88" s="44"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="45"/>
+      <c r="M88" s="45"/>
+      <c r="N88" s="46"/>
+      <c r="O88" s="43"/>
       <c r="P88" s="1"/>
       <c r="Q88" s="13"/>
       <c r="R88" s="13"/>
@@ -3773,11 +3944,11 @@
       <c r="H89" s="37"/>
       <c r="I89" s="37"/>
       <c r="J89" s="38"/>
-      <c r="K89" s="45"/>
-      <c r="L89" s="46"/>
-      <c r="M89" s="46"/>
-      <c r="N89" s="47"/>
-      <c r="O89" s="44"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="45"/>
+      <c r="M89" s="45"/>
+      <c r="N89" s="46"/>
+      <c r="O89" s="43"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="13"/>
       <c r="R89" s="13"/>
@@ -3795,16 +3966,192 @@
       <c r="H90" s="37"/>
       <c r="I90" s="37"/>
       <c r="J90" s="38"/>
-      <c r="K90" s="45"/>
-      <c r="L90" s="46"/>
-      <c r="M90" s="46"/>
-      <c r="N90" s="47"/>
-      <c r="O90" s="44"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="45"/>
+      <c r="M90" s="45"/>
+      <c r="N90" s="46"/>
+      <c r="O90" s="43"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="13"/>
       <c r="R90" s="13"/>
       <c r="S90" s="13"/>
       <c r="T90" s="2"/>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="44"/>
+      <c r="L91" s="45"/>
+      <c r="M91" s="45"/>
+      <c r="N91" s="46"/>
+      <c r="O91" s="43"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="13"/>
+      <c r="R91" s="13"/>
+      <c r="S91" s="13"/>
+      <c r="T91" s="2"/>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92" s="23"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="38"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="45"/>
+      <c r="M92" s="45"/>
+      <c r="N92" s="46"/>
+      <c r="O92" s="43"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="13"/>
+      <c r="R92" s="13"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="2"/>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A93" s="23"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="45"/>
+      <c r="M93" s="45"/>
+      <c r="N93" s="46"/>
+      <c r="O93" s="43"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="13"/>
+      <c r="R93" s="13"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="2"/>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94" s="23"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="38"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="45"/>
+      <c r="M94" s="45"/>
+      <c r="N94" s="46"/>
+      <c r="O94" s="43"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="2"/>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95" s="23"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="31"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="45"/>
+      <c r="M95" s="45"/>
+      <c r="N95" s="46"/>
+      <c r="O95" s="43"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="13"/>
+      <c r="R95" s="13"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="2"/>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A96" s="23"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="38"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="45"/>
+      <c r="M96" s="45"/>
+      <c r="N96" s="46"/>
+      <c r="O96" s="43"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="13"/>
+      <c r="R96" s="13"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="2"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97" s="23"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="31"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="44"/>
+      <c r="L97" s="45"/>
+      <c r="M97" s="45"/>
+      <c r="N97" s="46"/>
+      <c r="O97" s="43"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="13"/>
+      <c r="R97" s="13"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="2"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A98" s="23"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="31"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="38"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="45"/>
+      <c r="M98" s="45"/>
+      <c r="N98" s="46"/>
+      <c r="O98" s="43"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="13"/>
+      <c r="R98" s="13"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3816,31 +4163,31 @@
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A90</xm:sqref>
+          <xm:sqref>A2:A98</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K90</xm:sqref>
+          <xm:sqref>K2:K98</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L90</xm:sqref>
+          <xm:sqref>L2:L98</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$50</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M90</xm:sqref>
+          <xm:sqref>M2:M98</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O90</xm:sqref>
+          <xm:sqref>O2:O98</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Carga de contenidos de Ana María Lara
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/Escaleta_CS_09_03_CO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="236">
   <si>
     <t>Asignatura</t>
   </si>
@@ -723,12 +723,33 @@
   <si>
     <t>M101A</t>
   </si>
+  <si>
+    <t>http://aulaplaneta.planetasaber.com/encyclopedia/default.asp?idpack=10&amp;idpil=VI000466&amp;ruta=aulaplaneta&amp;DATA=liXdw0UWeePyPuT96hOWiTfqpXb%2b3YLTbbj%2btkCHHwY%3d</t>
+  </si>
+  <si>
+    <t>AUDIO ALVARO CEPEDA ZAMUDIO</t>
+  </si>
+  <si>
+    <t>SOLO SE VEN FOTOS</t>
+  </si>
+  <si>
+    <t>aparece para audio pero no para video</t>
+  </si>
+  <si>
+    <t>faltan audios y fotos.</t>
+  </si>
+  <si>
+    <t>LISTA</t>
+  </si>
+  <si>
+    <t>APARECE COMO F11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,8 +815,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -901,6 +930,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1136,10 +1177,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1233,13 +1275,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1266,18 +1318,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1580,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,97 +1667,97 @@
     <col min="22" max="16384" width="10.7109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="72"/>
-      <c r="O1" s="65" t="s">
+      <c r="N1" s="76"/>
+      <c r="O1" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="74" t="s">
+      <c r="Q1" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="76" t="s">
+      <c r="R1" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="74" t="s">
+      <c r="S1" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="75" t="s">
+      <c r="T1" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="74" t="s">
+      <c r="U1" s="65" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="68"/>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="71"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="3" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="74"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="65"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>85</v>
       </c>
@@ -1733,7 +1790,7 @@
       <c r="T3" s="15"/>
       <c r="U3" s="31"/>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>85</v>
       </c>
@@ -1794,7 +1851,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>85</v>
       </c>
@@ -1829,7 +1886,7 @@
       <c r="T5" s="16"/>
       <c r="U5" s="45"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
@@ -1864,7 +1921,7 @@
       <c r="T6" s="16"/>
       <c r="U6" s="45"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>85</v>
       </c>
@@ -1927,7 +1984,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>85</v>
       </c>
@@ -1962,7 +2019,7 @@
       <c r="T8" s="16"/>
       <c r="U8" s="45"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>85</v>
       </c>
@@ -1997,7 +2054,7 @@
       <c r="T9" s="16"/>
       <c r="U9" s="45"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>85</v>
       </c>
@@ -2060,7 +2117,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>85</v>
       </c>
@@ -2095,7 +2152,7 @@
       <c r="T11" s="16"/>
       <c r="U11" s="45"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>85</v>
       </c>
@@ -2130,7 +2187,7 @@
       <c r="T12" s="16"/>
       <c r="U12" s="45"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>85</v>
       </c>
@@ -2165,7 +2222,7 @@
       <c r="T13" s="16"/>
       <c r="U13" s="45"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>85</v>
       </c>
@@ -2184,25 +2241,25 @@
       <c r="F14" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="79">
         <v>4</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="42" t="s">
+      <c r="L14" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="81" t="s">
         <v>63</v>
       </c>
       <c r="N14" s="2"/>
@@ -2227,8 +2284,11 @@
       <c r="U14" s="20" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V14" s="83" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>85</v>
       </c>
@@ -2245,25 +2305,25 @@
         <v>104</v>
       </c>
       <c r="F15" s="39"/>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="79">
         <v>5</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="80" t="s">
         <v>220</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="42" t="s">
+      <c r="L15" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="M15" s="2"/>
+      <c r="M15" s="81"/>
       <c r="N15" s="2"/>
       <c r="O15" s="43" t="s">
         <v>224</v>
@@ -2286,8 +2346,14 @@
       <c r="U15" s="20" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V15" s="86" t="s">
+        <v>232</v>
+      </c>
+      <c r="W15" s="84" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>85</v>
       </c>
@@ -2341,14 +2407,17 @@
       <c r="S16" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="T16" s="77" t="s">
+      <c r="T16" s="63" t="s">
         <v>225</v>
       </c>
       <c r="U16" s="20" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V16" s="87" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>85</v>
       </c>
@@ -2383,7 +2452,7 @@
       <c r="T17" s="16"/>
       <c r="U17" s="45"/>
     </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>85</v>
       </c>
@@ -2402,25 +2471,25 @@
       <c r="F18" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="79">
         <v>7</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="J18" s="80" t="s">
         <v>146</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="42" t="s">
+      <c r="L18" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="81" t="s">
         <v>63</v>
       </c>
       <c r="N18" s="2"/>
@@ -2445,8 +2514,11 @@
       <c r="U18" s="20" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V18" s="85" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>85</v>
       </c>
@@ -2508,8 +2580,11 @@
       <c r="U19" s="20" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V19" s="83" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>85</v>
       </c>
@@ -2571,8 +2646,11 @@
       <c r="U20" s="20" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V20" s="83" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>85</v>
       </c>
@@ -2607,7 +2685,7 @@
       <c r="T21" s="16"/>
       <c r="U21" s="45"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>85</v>
       </c>
@@ -2642,7 +2720,7 @@
       <c r="T22" s="16"/>
       <c r="U22" s="45"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>85</v>
       </c>
@@ -2677,7 +2755,7 @@
       <c r="T23" s="16"/>
       <c r="U23" s="45"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>85</v>
       </c>
@@ -2739,8 +2817,11 @@
       <c r="U24" s="20" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V24" s="83" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>85</v>
       </c>
@@ -2794,14 +2875,14 @@
       <c r="S25" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="T25" s="77" t="s">
+      <c r="T25" s="63" t="s">
         <v>226</v>
       </c>
       <c r="U25" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>85</v>
       </c>
@@ -2862,7 +2943,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>85</v>
       </c>
@@ -2923,7 +3004,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>85</v>
       </c>
@@ -2977,14 +3058,14 @@
       <c r="S28" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="T28" s="77" t="s">
+      <c r="T28" s="63" t="s">
         <v>199</v>
       </c>
       <c r="U28" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>85</v>
       </c>
@@ -3017,7 +3098,7 @@
       <c r="T29" s="16"/>
       <c r="U29" s="45"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>85</v>
       </c>
@@ -3078,7 +3159,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>85</v>
       </c>
@@ -3132,14 +3213,14 @@
       <c r="S31" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="T31" s="77" t="s">
+      <c r="T31" s="63" t="s">
         <v>210</v>
       </c>
       <c r="U31" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
         <v>85</v>
       </c>
@@ -3368,7 +3449,7 @@
       <c r="S35" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="T35" s="77" t="s">
+      <c r="T35" s="63" t="s">
         <v>227</v>
       </c>
       <c r="U35" s="20" t="s">
@@ -3640,12 +3721,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3660,9 +3735,18 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="W15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4194,7 +4278,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>

</xml_diff>